<commit_message>
aggiornata checklist e data.json dei test case
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/PS3/3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/PS3/3.0.0/report-checklist.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$383</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$380</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$380</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$383</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -303,13 +303,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:48:20Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11cf9b6dbb6c4ab3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.c8a5681e5c6e538766d0ac6a40a40fe267e5d9149907cd4c8e396ca83cc37d51.582fdcad09^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T11:43:55Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d8367d1f8ce2ea1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.c8a5681e5c6e538766d0ac6a40a40fe267e5d9149907cd4c8e396ca83cc37d51.5cf6f5dbdc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -326,13 +326,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:49:16Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a2f3afc11a87f8f9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.6e81eadb23cfbe0235327f05ac620a03f2b2c650a29ee9f8c04dd252e510916a.94486892fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T12:03:06Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09c7174c158b3507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.6e81eadb23cfbe0235327f05ac620a03f2b2c650a29ee9f8c04dd252e510916a.214911b45e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">NO</t>
@@ -349,13 +349,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:50:27Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5a9a1fb67aed0896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.6afa85f67e5a71c943f9a7fdd568f43f93676268969439390a96bbcb6f569bc4.986bd1ee0a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T12:07:14Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e67b58641adb2ac6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.6afa85f67e5a71c943f9a7fdd568f43f93676268969439390a96bbcb6f569bc4.b9c60722ac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Il test non è applicabile perché la soluzione software di pronto soccorso non traccia informazioni in merito a: section[@ID="Inquadramento_Clinico_Iniziale"]/component/section[@ID="Anamnesi"]/entry L'applicativo non gestisce il dato strutturato dell'anamnesi ,l'applicativo permette di inserire solo il blocco narrativo dell'anamnesi. ClinicalDocument/component/structuredBody/component/section[@ID="Inquadramento_Clinico_Iniziale"]/component/section[@ID="Anamnesi"]/entry/observation/entryRelationship - non gestita la codifica di tale informazione. ClinicalDocument/component/structuredBody/component/section[@ID="Inquadramento_Clinico_Iniziale"]/component/section[@ID="Allergie"]/entry L'applicativo non gestisce il dato strutturato dell'allergia ,l'applicativo permette di inserire solo il blocco narrativo dell'allergia. ClinicalDocument/component/structuredBody/component/section[@ID="Dimissione"]/entry/act/entryRelationship/encounter/id - Identifica il codice nosologico il codice non è disponibile all'atto della dimissione/ricovero/trasferimento del paziente. ClinicalDocument/component/structuredBody/component/section[@ID="Piano_Cura_Dimissione"]/entry- L'applicativo non gestisce il dato strutturato del piano di cura alla dimissione ,l'applicativo permette di inserire solo il blocco narrativo piano di cura alla dimissione. L'eventuale produzione di NRE a corredo del piano di cura alla dimisisone non è gestita dall'applicativo. ClinicalDocument/component/structuredBody/component/section[@ID="Terapia_Farmacologica_Dimissione"]/entry - L'applicativo non gestisce il dato strutturato della terapia farmacologica alla dimissione,l'applicativo permette di inserire solo il blocco narrativo della terapia farmacologica alla dimissione. L'eventuale produzione di NRE a corredo della terapia farmacologica alla dimissione non è gestita dall'applicativo. ClinicalDocument/component/structuredBody/component/section[@ID="Terapia_Farmacologica_Dimissione"]/entry/substanceAdministration/consumable/manufacturedProduct/manufacturedMaterial - Contiene informazioni relative alla tipologia di farmaco oggetto della terapia. L'informazione dei farmaci indicati per la terapia farmacologica alla dimissione sono indicati in un blocco narrativo e l'applicativo non gestisce la codifica dei farmaci. ClinicalDocument/component/structuredBody/component/section[@ID="Complicanze"] L'informazione non è tracciata in un campo dedicato</t>
@@ -369,13 +369,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:51:20Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7af768a3fdc9cdea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.157a5ee7f8c9d19fcc827d62bf104578955fdbcabd109a9acef264fc8b304eb6.da9a9b0abb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T12:09:35Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0c5cf3d3955f022f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.157a5ee7f8c9d19fcc827d62bf104578955fdbcabd109a9acef264fc8b304eb6.636e893cb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section[@ID="Inquadramento_Clinico_Iniziale"]/component/section[@ID="Anamnesi"]/entry L'applicativo non gestisce il dato strutturato dell'anamnesi ,l'applicativo permette di inserire solo il blocco narrativo dell'anamnesi.  ClinicalDocument/component/structuredBody/component/section[@ID="Inquadramento_Clinico_Iniziale"]/component/section[@ID="Allergie"]/entry/act L'applicativo non gestisce il dato strutturato dell'allergia ,l'applicativo permette di inserire solo il blocco narrativo dell'allergia.  ClinicalDocument/component/structuredBody/component/section[@ID="Complicanze"] L'informazione non è tracciata in un campo dedicato  ClinicalDocument/component/structuredBody/component/section[@ID="Parametri_Vitali"]/entry L'applicativo non gestisce la codifica dei parametri vitali rilevati  ClinicalDocument/component/structuredBody/component/section[@ID="Terapia_Farmacologica_in_Pronto_Soccorso"]/entry L'applicativo non gestisce il dato strutturato della terapia farmacologica in PS,l'applicativo permette di inserire solo il blocco narrativo della terapia farmacologica in PS.   ClinicalDocument/component/structuredBody/component/section[@ID="Piano_Cura_Dimissione"]/entry L'applicativo non gestisce il dato strutturato del piano di cura alla dimissione ,l'applicativo permette di inserire solo il blocco narrativo piano di cura alla dimissione. L'eventuale produzione di NRE a corredo del piano di cura alla dimisisone non è gestita dall'applicativo.  ClinicalDocument/component/structuredBody/component/section[@ID="Terapia_Farmacologica_Dimissione"]/entry - L'applicativo non gestisce il dato strutturato della terapia farmacologica alla dimissione,l'applicativo permette di inserire solo il blocco narrativo della terapia farmacologica alla dimissione. L'eventuale produzione di NRE a corredo della terapia farmacologica alla dimissione non è gestita dall'applicativo.  ClinicalDocument/component/structuredBody/component/section[@ID="Terapia_Farmacologica_Dimissione"]/entry/substanceAdministration/consumable/manufacturedProduct/manufacturedMaterial - Contiene informazioni relative alla tipologia di farmaco oggetto della terapia. L'informazione dei farmaci indicati per la terapia farmacologica alla dimissione sono indicati in un blocco narrativo e l'applicativo non gestisce la codifica dei farmaci.</t>
@@ -547,13 +547,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:52:57Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a804ae871c3058a1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.9851983b07872443e42a371abc7a36efe071353589131802b7936beab1ef1fc5.c208e28a72^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T12:16:13Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17dab019953a274a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.c8a5681e5c6e538766d0ac6a40a40fe267e5d9149907cd4c8e396ca83cc37d51.3b1910e93a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico.[ERRORE-12| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
@@ -569,13 +569,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:57:12Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4d3bd08dde75a89a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.9851983b07872443e42a371abc7a36efe071353589131802b7936beab1ef1fc5.8d9eeef7bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T12:19:47Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd1a341ad4d93f4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.c8a5681e5c6e538766d0ac6a40a40fe267e5d9149907cd4c8e396ca83cc37d51.ffb1cb45ac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico.[ERRORE-15| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
@@ -793,13 +793,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-05T11:46:41Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94fe3e723f61f42a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.c8df1c27ecf7136c1f08524445486fef097259ed62114bb2d5a85d8b40d43eee.3dde0beeee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-10-12T12:23:39Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3f9f2723455f2e45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.c8df1c27ecf7136c1f08524445486fef097259ed62114bb2d5a85d8b40d43eee.586483b834^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -1466,7 +1466,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2540,7 +2540,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3646,15 +3646,15 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E134" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G393" activeCellId="0" sqref="G393"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B131" activeCellId="0" sqref="B131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="33.14"/>
@@ -4382,7 +4382,7 @@
         <v>54</v>
       </c>
       <c r="F31" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>55</v>
@@ -4426,7 +4426,7 @@
         <v>61</v>
       </c>
       <c r="F32" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>62</v>
@@ -4472,7 +4472,7 @@
         <v>68</v>
       </c>
       <c r="F33" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G33" s="28" t="s">
         <v>69</v>
@@ -4518,7 +4518,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>75</v>
@@ -6801,7 +6801,7 @@
         <v>100</v>
       </c>
       <c r="F132" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G132" s="28" t="s">
         <v>101</v>
@@ -6855,7 +6855,7 @@
         <v>107</v>
       </c>
       <c r="F133" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G133" s="28" t="s">
         <v>108</v>
@@ -12640,7 +12640,7 @@
         <v>172</v>
       </c>
       <c r="F380" s="27" t="n">
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="G380" s="28" t="s">
         <v>173</v>
@@ -17385,7 +17385,7 @@
       <c r="T1000" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T383">
+  <autoFilter ref="A9:T380">
     <filterColumn colId="2">
       <customFilters and="true">
         <customFilter operator="equal" val="VPS"/>
@@ -17433,7 +17433,7 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -19115,7 +19115,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>

</xml_diff>

<commit_message>
modificato gestione errore ID 51,125 e 126
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/PS3/3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/PS3/3.0.0/report-checklist.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$383</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$380</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$380</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$383</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -506,7 +506,7 @@
     <t xml:space="preserve">Non è stato possibile validare il documento ,riprovare</t>
   </si>
   <si>
-    <t xml:space="preserve">si ritenta la validazione</t>
+    <t xml:space="preserve">L'operazione di retry viene eseguita manualmente dall'operatore in backoffice</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_VPS_CT5_KO</t>
@@ -559,7 +559,7 @@
     <t xml:space="preserve">Errore semantico.[ERRORE-12| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
   </si>
   <si>
-    <t xml:space="preserve">L’operatore corregge i dati dell’anagrafica paziente ed effettua una nuova validazione</t>
+    <t xml:space="preserve">L’operatore viene avvisato dell’errore legato all’anagrafica del paziente,l’applicativo permette di interrompere l’operazione di validazione e  l’operatore può corregge i dati dell’anagrafica paziente ed effettua un nuovo tentativo di validazione</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_VPS_CT9_KO</t>
@@ -991,7 +991,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1061,6 +1061,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1202,7 +1208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1339,11 +1345,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1466,7 +1476,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2540,7 +2550,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3646,11 +3656,11 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G153" activeCellId="0" sqref="G153"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P132" activeCellId="0" sqref="P132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -4365,7 +4375,7 @@
       <c r="S30" s="31"/>
       <c r="T30" s="32"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="n">
         <v>24</v>
       </c>
@@ -4409,7 +4419,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="n">
         <v>25</v>
       </c>
@@ -4455,7 +4465,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="n">
         <v>26</v>
       </c>
@@ -4501,7 +4511,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="24" t="n">
         <v>27</v>
       </c>
@@ -4701,7 +4711,7 @@
       <c r="S41" s="31"/>
       <c r="T41" s="32"/>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="24" t="n">
         <v>35</v>
       </c>
@@ -4893,7 +4903,7 @@
       <c r="S49" s="31"/>
       <c r="T49" s="32"/>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="24" t="n">
         <v>43</v>
       </c>
@@ -6671,7 +6681,7 @@
       <c r="S128" s="31"/>
       <c r="T128" s="32"/>
     </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="24" t="n">
         <v>122</v>
       </c>
@@ -6708,7 +6718,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="24" t="n">
         <v>123</v>
       </c>
@@ -6746,7 +6756,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="24" t="n">
         <v>124</v>
       </c>
@@ -6882,7 +6892,7 @@
       <c r="O133" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="P133" s="29" t="s">
+      <c r="P133" s="34" t="s">
         <v>105</v>
       </c>
       <c r="Q133" s="29"/>
@@ -6892,7 +6902,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="24" t="n">
         <v>127</v>
       </c>
@@ -6930,7 +6940,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="24" t="n">
         <v>128</v>
       </c>
@@ -6968,7 +6978,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="24" t="n">
         <v>129</v>
       </c>
@@ -6991,7 +7001,7 @@
       <c r="J136" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K136" s="34" t="s">
+      <c r="K136" s="35" t="s">
         <v>120</v>
       </c>
       <c r="L136" s="29"/>
@@ -7006,7 +7016,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="24" t="n">
         <v>130</v>
       </c>
@@ -7044,7 +7054,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="24" t="n">
         <v>131</v>
       </c>
@@ -7082,7 +7092,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="24" t="n">
         <v>132</v>
       </c>
@@ -7120,7 +7130,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="24" t="n">
         <v>133</v>
       </c>
@@ -7158,7 +7168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="24" t="n">
         <v>134</v>
       </c>
@@ -7196,7 +7206,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="24" t="n">
         <v>135</v>
       </c>
@@ -7234,7 +7244,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="24" t="n">
         <v>136</v>
       </c>
@@ -7257,7 +7267,7 @@
       <c r="J143" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K143" s="35" t="s">
+      <c r="K143" s="36" t="s">
         <v>141</v>
       </c>
       <c r="L143" s="29"/>
@@ -7272,7 +7282,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="24" t="n">
         <v>137</v>
       </c>
@@ -7310,7 +7320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="24" t="n">
         <v>138</v>
       </c>
@@ -7333,7 +7343,7 @@
       <c r="J145" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K145" s="34" t="s">
+      <c r="K145" s="35" t="s">
         <v>147</v>
       </c>
       <c r="L145" s="29"/>
@@ -7348,7 +7358,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="24" t="n">
         <v>139</v>
       </c>
@@ -7371,7 +7381,7 @@
       <c r="J146" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K146" s="34" t="s">
+      <c r="K146" s="35" t="s">
         <v>150</v>
       </c>
       <c r="L146" s="29"/>
@@ -7386,7 +7396,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="24" t="n">
         <v>140</v>
       </c>
@@ -7409,7 +7419,7 @@
       <c r="J147" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K147" s="35" t="s">
+      <c r="K147" s="36" t="s">
         <v>153</v>
       </c>
       <c r="L147" s="29"/>
@@ -7424,7 +7434,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="24" t="n">
         <v>141</v>
       </c>
@@ -7447,7 +7457,7 @@
       <c r="J148" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K148" s="34" t="s">
+      <c r="K148" s="35" t="s">
         <v>156</v>
       </c>
       <c r="L148" s="29"/>
@@ -7462,7 +7472,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="24" t="n">
         <v>142</v>
       </c>
@@ -7485,7 +7495,7 @@
       <c r="J149" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K149" s="34" t="s">
+      <c r="K149" s="35" t="s">
         <v>159</v>
       </c>
       <c r="L149" s="29"/>
@@ -7500,7 +7510,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="24" t="n">
         <v>143</v>
       </c>
@@ -7538,7 +7548,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="24" t="n">
         <v>144</v>
       </c>
@@ -7576,7 +7586,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="24" t="n">
         <v>145</v>
       </c>
@@ -7599,7 +7609,7 @@
       <c r="J152" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K152" s="35" t="s">
+      <c r="K152" s="36" t="s">
         <v>167</v>
       </c>
       <c r="L152" s="29"/>
@@ -7614,7 +7624,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="24" t="n">
         <v>146</v>
       </c>
@@ -12623,7 +12633,7 @@
       <c r="S379" s="31"/>
       <c r="T379" s="32"/>
     </row>
-    <row r="380" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A380" s="24" t="n">
         <v>373</v>
       </c>
@@ -17385,11 +17395,18 @@
       <c r="T1000" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T383">
+  <autoFilter ref="A9:T380">
     <filterColumn colId="2">
       <customFilters and="true">
         <customFilter operator="equal" val="VPS"/>
       </customFilters>
+    </filterColumn>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="125"/>
+        <filter val="126"/>
+        <filter val="51"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="4">
@@ -17433,7 +17450,7 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -17464,10 +17481,10 @@
       <c r="B2" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>181</v>
       </c>
     </row>
@@ -17478,10 +17495,10 @@
       <c r="B3" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>184</v>
       </c>
     </row>
@@ -17492,10 +17509,10 @@
       <c r="B4" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>187</v>
       </c>
     </row>
@@ -17506,10 +17523,10 @@
       <c r="B5" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>190</v>
       </c>
     </row>
@@ -17520,10 +17537,10 @@
       <c r="B6" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>193</v>
       </c>
     </row>
@@ -17534,10 +17551,10 @@
       <c r="B7" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="38" t="s">
         <v>195</v>
       </c>
     </row>
@@ -17548,10 +17565,10 @@
       <c r="B8" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>198</v>
       </c>
     </row>
@@ -17562,10 +17579,10 @@
       <c r="B9" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="38" t="s">
         <v>201</v>
       </c>
     </row>
@@ -17576,10 +17593,10 @@
       <c r="B10" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="37" t="s">
         <v>204</v>
       </c>
     </row>
@@ -17590,10 +17607,10 @@
       <c r="B11" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C11" s="36" t="n">
+      <c r="C11" s="37" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="37" t="s">
         <v>206</v>
       </c>
     </row>
@@ -17604,10 +17621,10 @@
       <c r="B12" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="36" t="n">
+      <c r="C12" s="37" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="37" t="s">
         <v>207</v>
       </c>
     </row>
@@ -17618,10 +17635,10 @@
       <c r="B13" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="36" t="n">
+      <c r="C13" s="37" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="38" t="s">
         <v>208</v>
       </c>
     </row>
@@ -17632,10 +17649,10 @@
       <c r="B14" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C14" s="36" t="n">
+      <c r="C14" s="37" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="37" t="s">
         <v>209</v>
       </c>
     </row>
@@ -17646,10 +17663,10 @@
       <c r="B15" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C15" s="36" t="n">
+      <c r="C15" s="37" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="38" t="s">
         <v>210</v>
       </c>
     </row>
@@ -17660,10 +17677,10 @@
       <c r="B16" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C16" s="36" t="n">
+      <c r="C16" s="37" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -17674,10 +17691,10 @@
       <c r="B17" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C17" s="36" t="n">
+      <c r="C17" s="37" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="38" t="s">
         <v>212</v>
       </c>
     </row>
@@ -17688,10 +17705,10 @@
       <c r="B18" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C18" s="36" t="n">
+      <c r="C18" s="37" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="38" t="s">
         <v>213</v>
       </c>
     </row>
@@ -17702,10 +17719,10 @@
       <c r="B19" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="36" t="n">
+      <c r="C19" s="37" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="37" t="s">
         <v>215</v>
       </c>
     </row>
@@ -17716,10 +17733,10 @@
       <c r="B20" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="36" t="n">
+      <c r="C20" s="37" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="37" t="s">
         <v>216</v>
       </c>
     </row>
@@ -17730,10 +17747,10 @@
       <c r="B21" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C21" s="36" t="n">
+      <c r="C21" s="37" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="38" t="s">
         <v>217</v>
       </c>
     </row>
@@ -17744,10 +17761,10 @@
       <c r="B22" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C22" s="36" t="n">
+      <c r="C22" s="37" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="37" t="s">
         <v>218</v>
       </c>
     </row>
@@ -17758,10 +17775,10 @@
       <c r="B23" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C23" s="36" t="n">
+      <c r="C23" s="37" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="38" t="s">
         <v>219</v>
       </c>
     </row>
@@ -17772,10 +17789,10 @@
       <c r="B24" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C24" s="36" t="n">
+      <c r="C24" s="37" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="38" t="s">
         <v>220</v>
       </c>
     </row>
@@ -17786,10 +17803,10 @@
       <c r="B25" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C25" s="36" t="n">
+      <c r="C25" s="37" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="38" t="s">
         <v>221</v>
       </c>
     </row>
@@ -17800,10 +17817,10 @@
       <c r="B26" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C26" s="36" t="n">
+      <c r="C26" s="37" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="38" t="s">
         <v>222</v>
       </c>
     </row>
@@ -17814,10 +17831,10 @@
       <c r="B27" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C27" s="36" t="n">
+      <c r="C27" s="37" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="37" t="s">
         <v>224</v>
       </c>
     </row>
@@ -17828,10 +17845,10 @@
       <c r="B28" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C28" s="36" t="n">
+      <c r="C28" s="37" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="37" t="s">
         <v>225</v>
       </c>
     </row>
@@ -17842,10 +17859,10 @@
       <c r="B29" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C29" s="36" t="n">
+      <c r="C29" s="37" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="39" t="s">
         <v>226</v>
       </c>
     </row>
@@ -17856,10 +17873,10 @@
       <c r="B30" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C30" s="36" t="n">
+      <c r="C30" s="37" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="37" t="s">
         <v>227</v>
       </c>
     </row>
@@ -17870,10 +17887,10 @@
       <c r="B31" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C31" s="36" t="n">
+      <c r="C31" s="37" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="38" t="s">
         <v>228</v>
       </c>
     </row>
@@ -17884,10 +17901,10 @@
       <c r="B32" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="36" t="n">
+      <c r="C32" s="37" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="38" t="s">
         <v>229</v>
       </c>
     </row>
@@ -17898,10 +17915,10 @@
       <c r="B33" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C33" s="36" t="n">
+      <c r="C33" s="37" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="38" t="s">
         <v>230</v>
       </c>
     </row>
@@ -17912,10 +17929,10 @@
       <c r="B34" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C34" s="36" t="n">
+      <c r="C34" s="37" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="38" t="s">
         <v>231</v>
       </c>
     </row>
@@ -17926,10 +17943,10 @@
       <c r="B35" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C35" s="36" t="n">
+      <c r="C35" s="37" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="36" t="n">
+      <c r="D35" s="37" t="n">
         <v>204</v>
       </c>
     </row>
@@ -17940,10 +17957,10 @@
       <c r="B36" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C36" s="36" t="n">
+      <c r="C36" s="37" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="36" t="n">
+      <c r="D36" s="37" t="n">
         <v>220</v>
       </c>
     </row>
@@ -17954,10 +17971,10 @@
       <c r="B37" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C37" s="36" t="n">
+      <c r="C37" s="37" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="37" t="n">
+      <c r="D37" s="38" t="n">
         <v>236</v>
       </c>
     </row>
@@ -17968,10 +17985,10 @@
       <c r="B38" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C38" s="36" t="n">
+      <c r="C38" s="37" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="36" t="n">
+      <c r="D38" s="37" t="n">
         <v>252</v>
       </c>
     </row>
@@ -17982,10 +17999,10 @@
       <c r="B39" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="36" t="n">
+      <c r="C39" s="37" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="37" t="n">
+      <c r="D39" s="38" t="n">
         <v>268</v>
       </c>
     </row>
@@ -17996,10 +18013,10 @@
       <c r="B40" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C40" s="36" t="n">
+      <c r="C40" s="37" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="37" t="n">
+      <c r="D40" s="38" t="n">
         <v>284</v>
       </c>
     </row>
@@ -18010,10 +18027,10 @@
       <c r="B41" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C41" s="36" t="n">
+      <c r="C41" s="37" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="37" t="n">
+      <c r="D41" s="38" t="n">
         <v>300</v>
       </c>
     </row>
@@ -18024,10 +18041,10 @@
       <c r="B42" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C42" s="36" t="n">
+      <c r="C42" s="37" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="37" t="n">
+      <c r="D42" s="38" t="n">
         <v>316</v>
       </c>
     </row>
@@ -18038,10 +18055,10 @@
       <c r="B43" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C43" s="36" t="n">
+      <c r="C43" s="37" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="36" t="n">
+      <c r="D43" s="37" t="n">
         <v>207</v>
       </c>
     </row>
@@ -18052,10 +18069,10 @@
       <c r="B44" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C44" s="36" t="n">
+      <c r="C44" s="37" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="36" t="n">
+      <c r="D44" s="37" t="n">
         <v>223</v>
       </c>
     </row>
@@ -18066,10 +18083,10 @@
       <c r="B45" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="36" t="n">
+      <c r="C45" s="37" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="37" t="n">
+      <c r="D45" s="38" t="n">
         <v>239</v>
       </c>
     </row>
@@ -18080,10 +18097,10 @@
       <c r="B46" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C46" s="36" t="n">
+      <c r="C46" s="37" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="36" t="n">
+      <c r="D46" s="37" t="n">
         <v>255</v>
       </c>
     </row>
@@ -18094,10 +18111,10 @@
       <c r="B47" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C47" s="36" t="n">
+      <c r="C47" s="37" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="37" t="n">
+      <c r="D47" s="38" t="n">
         <v>271</v>
       </c>
     </row>
@@ -18108,10 +18125,10 @@
       <c r="B48" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C48" s="36" t="n">
+      <c r="C48" s="37" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="37" t="n">
+      <c r="D48" s="38" t="n">
         <v>287</v>
       </c>
     </row>
@@ -18122,10 +18139,10 @@
       <c r="B49" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C49" s="36" t="n">
+      <c r="C49" s="37" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="37" t="n">
+      <c r="D49" s="38" t="n">
         <v>303</v>
       </c>
     </row>
@@ -18136,10 +18153,10 @@
       <c r="B50" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C50" s="36" t="n">
+      <c r="C50" s="37" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="37" t="n">
+      <c r="D50" s="38" t="n">
         <v>319</v>
       </c>
     </row>
@@ -19115,7 +19132,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -19124,32 +19141,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
modificata gestione errore ID 51,125 e 126
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/PS3/3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/PS3/3.0.0/report-checklist.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$380</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$383</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$383</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$380</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -991,7 +991,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1061,12 +1061,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1208,7 +1202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1345,15 +1339,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1476,7 +1466,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2550,7 +2540,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3656,11 +3646,11 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P132" activeCellId="0" sqref="P132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -4375,7 +4365,7 @@
       <c r="S30" s="31"/>
       <c r="T30" s="32"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="n">
         <v>24</v>
       </c>
@@ -4419,7 +4409,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="n">
         <v>25</v>
       </c>
@@ -4465,7 +4455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="n">
         <v>26</v>
       </c>
@@ -4511,7 +4501,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="24" t="n">
         <v>27</v>
       </c>
@@ -4711,7 +4701,7 @@
       <c r="S41" s="31"/>
       <c r="T41" s="32"/>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="24" t="n">
         <v>35</v>
       </c>
@@ -4903,7 +4893,7 @@
       <c r="S49" s="31"/>
       <c r="T49" s="32"/>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="24" t="n">
         <v>43</v>
       </c>
@@ -6681,7 +6671,7 @@
       <c r="S128" s="31"/>
       <c r="T128" s="32"/>
     </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="24" t="n">
         <v>122</v>
       </c>
@@ -6718,7 +6708,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="24" t="n">
         <v>123</v>
       </c>
@@ -6756,7 +6746,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="24" t="n">
         <v>124</v>
       </c>
@@ -6892,7 +6882,7 @@
       <c r="O133" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="P133" s="34" t="s">
+      <c r="P133" s="29" t="s">
         <v>105</v>
       </c>
       <c r="Q133" s="29"/>
@@ -6902,7 +6892,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="24" t="n">
         <v>127</v>
       </c>
@@ -6940,7 +6930,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="24" t="n">
         <v>128</v>
       </c>
@@ -6978,7 +6968,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="24" t="n">
         <v>129</v>
       </c>
@@ -7001,7 +6991,7 @@
       <c r="J136" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K136" s="35" t="s">
+      <c r="K136" s="34" t="s">
         <v>120</v>
       </c>
       <c r="L136" s="29"/>
@@ -7016,7 +7006,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="24" t="n">
         <v>130</v>
       </c>
@@ -7054,7 +7044,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="24" t="n">
         <v>131</v>
       </c>
@@ -7092,7 +7082,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="24" t="n">
         <v>132</v>
       </c>
@@ -7130,7 +7120,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="24" t="n">
         <v>133</v>
       </c>
@@ -7168,7 +7158,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="24" t="n">
         <v>134</v>
       </c>
@@ -7206,7 +7196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="24" t="n">
         <v>135</v>
       </c>
@@ -7244,7 +7234,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="24" t="n">
         <v>136</v>
       </c>
@@ -7267,7 +7257,7 @@
       <c r="J143" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K143" s="36" t="s">
+      <c r="K143" s="35" t="s">
         <v>141</v>
       </c>
       <c r="L143" s="29"/>
@@ -7282,7 +7272,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="24" t="n">
         <v>137</v>
       </c>
@@ -7320,7 +7310,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="24" t="n">
         <v>138</v>
       </c>
@@ -7343,7 +7333,7 @@
       <c r="J145" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K145" s="35" t="s">
+      <c r="K145" s="34" t="s">
         <v>147</v>
       </c>
       <c r="L145" s="29"/>
@@ -7358,7 +7348,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="24" t="n">
         <v>139</v>
       </c>
@@ -7381,7 +7371,7 @@
       <c r="J146" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K146" s="35" t="s">
+      <c r="K146" s="34" t="s">
         <v>150</v>
       </c>
       <c r="L146" s="29"/>
@@ -7396,7 +7386,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="24" t="n">
         <v>140</v>
       </c>
@@ -7419,7 +7409,7 @@
       <c r="J147" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K147" s="36" t="s">
+      <c r="K147" s="35" t="s">
         <v>153</v>
       </c>
       <c r="L147" s="29"/>
@@ -7434,7 +7424,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="24" t="n">
         <v>141</v>
       </c>
@@ -7457,7 +7447,7 @@
       <c r="J148" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K148" s="35" t="s">
+      <c r="K148" s="34" t="s">
         <v>156</v>
       </c>
       <c r="L148" s="29"/>
@@ -7472,7 +7462,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="24" t="n">
         <v>142</v>
       </c>
@@ -7495,7 +7485,7 @@
       <c r="J149" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K149" s="35" t="s">
+      <c r="K149" s="34" t="s">
         <v>159</v>
       </c>
       <c r="L149" s="29"/>
@@ -7510,7 +7500,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="24" t="n">
         <v>143</v>
       </c>
@@ -7548,7 +7538,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="24" t="n">
         <v>144</v>
       </c>
@@ -7586,7 +7576,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="24" t="n">
         <v>145</v>
       </c>
@@ -7609,7 +7599,7 @@
       <c r="J152" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K152" s="36" t="s">
+      <c r="K152" s="35" t="s">
         <v>167</v>
       </c>
       <c r="L152" s="29"/>
@@ -7624,7 +7614,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="24" t="n">
         <v>146</v>
       </c>
@@ -12633,7 +12623,7 @@
       <c r="S379" s="31"/>
       <c r="T379" s="32"/>
     </row>
-    <row r="380" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A380" s="24" t="n">
         <v>373</v>
       </c>
@@ -17395,18 +17385,11 @@
       <c r="T1000" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T380">
+  <autoFilter ref="A9:T383">
     <filterColumn colId="2">
       <customFilters and="true">
         <customFilter operator="equal" val="VPS"/>
       </customFilters>
-    </filterColumn>
-    <filterColumn colId="0">
-      <filters>
-        <filter val="125"/>
-        <filter val="126"/>
-        <filter val="51"/>
-      </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="4">
@@ -17450,7 +17433,7 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -17481,10 +17464,10 @@
       <c r="B2" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>181</v>
       </c>
     </row>
@@ -17495,10 +17478,10 @@
       <c r="B3" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="36" t="s">
         <v>184</v>
       </c>
     </row>
@@ -17509,10 +17492,10 @@
       <c r="B4" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>187</v>
       </c>
     </row>
@@ -17523,10 +17506,10 @@
       <c r="B5" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="36" t="s">
         <v>190</v>
       </c>
     </row>
@@ -17537,10 +17520,10 @@
       <c r="B6" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="37" t="s">
         <v>193</v>
       </c>
     </row>
@@ -17551,10 +17534,10 @@
       <c r="B7" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="37" t="s">
         <v>195</v>
       </c>
     </row>
@@ -17565,10 +17548,10 @@
       <c r="B8" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>198</v>
       </c>
     </row>
@@ -17579,10 +17562,10 @@
       <c r="B9" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="37" t="s">
         <v>201</v>
       </c>
     </row>
@@ -17593,10 +17576,10 @@
       <c r="B10" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>204</v>
       </c>
     </row>
@@ -17607,10 +17590,10 @@
       <c r="B11" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C11" s="37" t="n">
+      <c r="C11" s="36" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
         <v>206</v>
       </c>
     </row>
@@ -17621,10 +17604,10 @@
       <c r="B12" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="37" t="n">
+      <c r="C12" s="36" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="36" t="s">
         <v>207</v>
       </c>
     </row>
@@ -17635,10 +17618,10 @@
       <c r="B13" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="37" t="n">
+      <c r="C13" s="36" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>208</v>
       </c>
     </row>
@@ -17649,10 +17632,10 @@
       <c r="B14" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C14" s="37" t="n">
+      <c r="C14" s="36" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="36" t="s">
         <v>209</v>
       </c>
     </row>
@@ -17663,10 +17646,10 @@
       <c r="B15" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C15" s="37" t="n">
+      <c r="C15" s="36" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="37" t="s">
         <v>210</v>
       </c>
     </row>
@@ -17677,10 +17660,10 @@
       <c r="B16" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C16" s="37" t="n">
+      <c r="C16" s="36" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="37" t="s">
         <v>211</v>
       </c>
     </row>
@@ -17691,10 +17674,10 @@
       <c r="B17" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C17" s="37" t="n">
+      <c r="C17" s="36" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="37" t="s">
         <v>212</v>
       </c>
     </row>
@@ -17705,10 +17688,10 @@
       <c r="B18" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C18" s="37" t="n">
+      <c r="C18" s="36" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="37" t="s">
         <v>213</v>
       </c>
     </row>
@@ -17719,10 +17702,10 @@
       <c r="B19" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="37" t="n">
+      <c r="C19" s="36" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="36" t="s">
         <v>215</v>
       </c>
     </row>
@@ -17733,10 +17716,10 @@
       <c r="B20" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="37" t="n">
+      <c r="C20" s="36" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="36" t="s">
         <v>216</v>
       </c>
     </row>
@@ -17747,10 +17730,10 @@
       <c r="B21" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C21" s="37" t="n">
+      <c r="C21" s="36" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="37" t="s">
         <v>217</v>
       </c>
     </row>
@@ -17761,10 +17744,10 @@
       <c r="B22" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C22" s="37" t="n">
+      <c r="C22" s="36" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="36" t="s">
         <v>218</v>
       </c>
     </row>
@@ -17775,10 +17758,10 @@
       <c r="B23" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C23" s="37" t="n">
+      <c r="C23" s="36" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="37" t="s">
         <v>219</v>
       </c>
     </row>
@@ -17789,10 +17772,10 @@
       <c r="B24" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C24" s="37" t="n">
+      <c r="C24" s="36" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="37" t="s">
         <v>220</v>
       </c>
     </row>
@@ -17803,10 +17786,10 @@
       <c r="B25" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C25" s="37" t="n">
+      <c r="C25" s="36" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="37" t="s">
         <v>221</v>
       </c>
     </row>
@@ -17817,10 +17800,10 @@
       <c r="B26" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C26" s="37" t="n">
+      <c r="C26" s="36" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="37" t="s">
         <v>222</v>
       </c>
     </row>
@@ -17831,10 +17814,10 @@
       <c r="B27" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C27" s="37" t="n">
+      <c r="C27" s="36" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="36" t="s">
         <v>224</v>
       </c>
     </row>
@@ -17845,10 +17828,10 @@
       <c r="B28" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C28" s="37" t="n">
+      <c r="C28" s="36" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="36" t="s">
         <v>225</v>
       </c>
     </row>
@@ -17859,10 +17842,10 @@
       <c r="B29" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C29" s="37" t="n">
+      <c r="C29" s="36" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="38" t="s">
         <v>226</v>
       </c>
     </row>
@@ -17873,10 +17856,10 @@
       <c r="B30" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C30" s="37" t="n">
+      <c r="C30" s="36" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="36" t="s">
         <v>227</v>
       </c>
     </row>
@@ -17887,10 +17870,10 @@
       <c r="B31" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C31" s="37" t="n">
+      <c r="C31" s="36" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="37" t="s">
         <v>228</v>
       </c>
     </row>
@@ -17901,10 +17884,10 @@
       <c r="B32" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="37" t="n">
+      <c r="C32" s="36" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="37" t="s">
         <v>229</v>
       </c>
     </row>
@@ -17915,10 +17898,10 @@
       <c r="B33" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C33" s="37" t="n">
+      <c r="C33" s="36" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="37" t="s">
         <v>230</v>
       </c>
     </row>
@@ -17929,10 +17912,10 @@
       <c r="B34" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C34" s="37" t="n">
+      <c r="C34" s="36" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="37" t="s">
         <v>231</v>
       </c>
     </row>
@@ -17943,10 +17926,10 @@
       <c r="B35" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C35" s="37" t="n">
+      <c r="C35" s="36" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="37" t="n">
+      <c r="D35" s="36" t="n">
         <v>204</v>
       </c>
     </row>
@@ -17957,10 +17940,10 @@
       <c r="B36" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C36" s="37" t="n">
+      <c r="C36" s="36" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="37" t="n">
+      <c r="D36" s="36" t="n">
         <v>220</v>
       </c>
     </row>
@@ -17971,10 +17954,10 @@
       <c r="B37" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C37" s="37" t="n">
+      <c r="C37" s="36" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="38" t="n">
+      <c r="D37" s="37" t="n">
         <v>236</v>
       </c>
     </row>
@@ -17985,10 +17968,10 @@
       <c r="B38" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C38" s="37" t="n">
+      <c r="C38" s="36" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="37" t="n">
+      <c r="D38" s="36" t="n">
         <v>252</v>
       </c>
     </row>
@@ -17999,10 +17982,10 @@
       <c r="B39" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="37" t="n">
+      <c r="C39" s="36" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="38" t="n">
+      <c r="D39" s="37" t="n">
         <v>268</v>
       </c>
     </row>
@@ -18013,10 +17996,10 @@
       <c r="B40" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C40" s="37" t="n">
+      <c r="C40" s="36" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="38" t="n">
+      <c r="D40" s="37" t="n">
         <v>284</v>
       </c>
     </row>
@@ -18027,10 +18010,10 @@
       <c r="B41" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C41" s="37" t="n">
+      <c r="C41" s="36" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="38" t="n">
+      <c r="D41" s="37" t="n">
         <v>300</v>
       </c>
     </row>
@@ -18041,10 +18024,10 @@
       <c r="B42" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C42" s="37" t="n">
+      <c r="C42" s="36" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="38" t="n">
+      <c r="D42" s="37" t="n">
         <v>316</v>
       </c>
     </row>
@@ -18055,10 +18038,10 @@
       <c r="B43" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C43" s="37" t="n">
+      <c r="C43" s="36" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="37" t="n">
+      <c r="D43" s="36" t="n">
         <v>207</v>
       </c>
     </row>
@@ -18069,10 +18052,10 @@
       <c r="B44" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C44" s="37" t="n">
+      <c r="C44" s="36" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="37" t="n">
+      <c r="D44" s="36" t="n">
         <v>223</v>
       </c>
     </row>
@@ -18083,10 +18066,10 @@
       <c r="B45" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="37" t="n">
+      <c r="C45" s="36" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="38" t="n">
+      <c r="D45" s="37" t="n">
         <v>239</v>
       </c>
     </row>
@@ -18097,10 +18080,10 @@
       <c r="B46" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C46" s="37" t="n">
+      <c r="C46" s="36" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="37" t="n">
+      <c r="D46" s="36" t="n">
         <v>255</v>
       </c>
     </row>
@@ -18111,10 +18094,10 @@
       <c r="B47" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C47" s="37" t="n">
+      <c r="C47" s="36" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="38" t="n">
+      <c r="D47" s="37" t="n">
         <v>271</v>
       </c>
     </row>
@@ -18125,10 +18108,10 @@
       <c r="B48" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C48" s="37" t="n">
+      <c r="C48" s="36" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="38" t="n">
+      <c r="D48" s="37" t="n">
         <v>287</v>
       </c>
     </row>
@@ -18139,10 +18122,10 @@
       <c r="B49" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C49" s="37" t="n">
+      <c r="C49" s="36" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="38" t="n">
+      <c r="D49" s="37" t="n">
         <v>303</v>
       </c>
     </row>
@@ -18153,10 +18136,10 @@
       <c r="B50" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C50" s="37" t="n">
+      <c r="C50" s="36" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="38" t="n">
+      <c r="D50" s="37" t="n">
         <v>319</v>
       </c>
     </row>
@@ -19132,7 +19115,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -19141,32 +19124,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>